<commit_message>
all file are pushed
</commit_message>
<xml_diff>
--- a/New Microsoft Office Excel Worksheet.xlsx
+++ b/New Microsoft Office Excel Worksheet.xlsx
@@ -11,8 +11,31 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="124519"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t xml:space="preserve">name </t>
+  </si>
+  <si>
+    <t>fName</t>
+  </si>
+  <si>
+    <t>cource</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kundan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">vinod  </t>
+  </si>
+  <si>
+    <t>dsa</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -342,12 +365,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>